<commit_message>
Backup before correcting Bmad upgrade issue
</commit_message>
<xml_diff>
--- a/2025-03-28 Using sextupole movers to control two-bunch pointing.xlsx
+++ b/2025-03-28 Using sextupole movers to control two-bunch pointing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmajik/Documents/SLAC/FACET2-Bmad-PyTao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{52E88D1B-959C-0C4B-923E-A2502817D68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63A13D5-4C83-B74D-A4D7-267B3890C4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18440" yWindow="4820" windowWidth="38120" windowHeight="19620" xr2:uid="{CD24CC5C-4DAA-064B-A554-3DA93A77CFA3}"/>
   </bookViews>
@@ -257,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -440,6 +440,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,7 +610,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -613,6 +619,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,7 +998,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,7 +1114,7 @@
       <c r="M2" s="1">
         <v>3.5424213668552603E-5</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="6">
         <v>9.8304246515239002E-2</v>
       </c>
       <c r="O2" s="2">
@@ -1175,7 +1182,7 @@
       <c r="N3" s="2">
         <v>3.31200275206962E-5</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="6">
         <v>0.100008098980833</v>
       </c>
       <c r="P3" s="2">
@@ -1243,7 +1250,7 @@
       <c r="O4" s="2">
         <v>-1.37611138481139E-3</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="6">
         <v>9.9654710981495698E-2</v>
       </c>
       <c r="Q4" s="2">
@@ -1305,13 +1312,13 @@
       <c r="N5" s="2">
         <v>4.8859293666739002E-3</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="5">
         <v>-5.0027946534639796E-3</v>
       </c>
       <c r="P5" s="2">
         <v>-1.0027463316945001E-3</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="6">
         <v>9.8457089044138399E-2</v>
       </c>
       <c r="R5" s="2">
@@ -1379,7 +1386,7 @@
       <c r="Q6" s="2">
         <v>1.3638780105025899E-3</v>
       </c>
-      <c r="R6" s="5">
+      <c r="R6" s="6">
         <v>0.100823494318246</v>
       </c>
       <c r="S6" s="2">
@@ -1447,7 +1454,7 @@
       <c r="R7" s="2">
         <v>7.6126872926597297E-4</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="6">
         <v>0.10064374951261799</v>
       </c>
       <c r="T7" s="2">
@@ -1515,7 +1522,7 @@
       <c r="S8" s="2">
         <v>-1.0037907414175899E-3</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="6">
         <v>0.10162947762484099</v>
       </c>
       <c r="U8" s="2">
@@ -1583,7 +1590,7 @@
       <c r="T9" s="2">
         <v>-2.0445726848965901E-3</v>
       </c>
-      <c r="U9" s="5">
+      <c r="U9" s="6">
         <v>0.103026731318443</v>
       </c>
     </row>

</xml_diff>